<commit_message>
subir todo de nuevo
</commit_message>
<xml_diff>
--- a/public/plantilla-emision-masiva_v2.xlsx
+++ b/public/plantilla-emision-masiva_v2.xlsx
@@ -5,10 +5,10 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Bendise\public\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\diego\OneDrive\Escritorio\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5BD26324-3E05-40EB-85A1-A3F78F03099B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{32BB2855-A92F-470B-A126-122E4B0C752A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -19,7 +19,7 @@
     <sheet name="Hoja3" sheetId="6" state="hidden" r:id="rId4"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">masiva_online!$D$7:$D$185</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">masiva_online!$D$7:$D$169</definedName>
   </definedNames>
   <calcPr calcId="191028"/>
   <extLst>
@@ -4310,8 +4310,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:T7"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
-      <selection activeCell="A8" sqref="A8:XFD8"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A3" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
+      <selection activeCell="C14" sqref="C14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4449,17 +4449,17 @@
     <mergeCell ref="D6:I6"/>
   </mergeCells>
   <phoneticPr fontId="18" type="noConversion"/>
-  <conditionalFormatting sqref="A8:T255">
+  <conditionalFormatting sqref="A8:T239">
     <cfRule type="expression" dxfId="0" priority="1" stopIfTrue="1">
       <formula>EXACT($A8,"EMISION")</formula>
     </cfRule>
   </conditionalFormatting>
   <dataValidations xWindow="1312" yWindow="583" count="20">
-    <dataValidation errorStyle="warning" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Formato rut " error="El formato  de rut debe ser así: _x000a_11.111.111-1" promptTitle="Formato" prompt="el formato de rut es: 11.111.111-1" sqref="D186:D1048576" xr:uid="{00000000-0002-0000-0000-000004000000}"/>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="Tipo de Fila" prompt="Se debe escoger si la fila que estoy ingresando es una EMISION con todos sus datos o una fila para agregar BULTOS" sqref="A186:A1048576" xr:uid="{00000000-0002-0000-0000-000007000000}">
+    <dataValidation errorStyle="warning" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Formato rut " error="El formato  de rut debe ser así: _x000a_11.111.111-1" promptTitle="Formato" prompt="el formato de rut es: 11.111.111-1" sqref="D170:D1048576" xr:uid="{00000000-0002-0000-0000-000004000000}"/>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="Tipo de Fila" prompt="Se debe escoger si la fila que estoy ingresando es una EMISION con todos sus datos o una fila para agregar BULTOS" sqref="A170:A1048576" xr:uid="{00000000-0002-0000-0000-000007000000}">
       <formula1>"EMISION, BULTO"</formula1>
     </dataValidation>
-    <dataValidation type="textLength" errorStyle="warning" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Formato rut " error="El formato  de rut debe ser así: _x000a_11.111.111-1" prompt="El rut debe ser ingresado con puntos y guión" sqref="D8:D185" xr:uid="{00000000-0002-0000-0000-000013000000}">
+    <dataValidation type="textLength" errorStyle="warning" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Formato rut " error="El formato  de rut debe ser así: _x000a_11.111.111-1" prompt="El rut debe ser ingresado con puntos y guión" sqref="D8:D169" xr:uid="{00000000-0002-0000-0000-000013000000}">
       <formula1>0</formula1>
       <formula2>12</formula2>
     </dataValidation>
@@ -4492,7 +4492,7 @@
       <formula1>0</formula1>
       <formula2>10000</formula2>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Escoge si la fila que vas a completar es una EMISION con todos los datos necesarios o una fila para agregar BULTOS en donde solo debes agregar medidas y peso" sqref="A8:A185" xr:uid="{00000000-0002-0000-0000-00001F000000}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Escoge si la fila que vas a completar es una EMISION con todos los datos necesarios o una fila para agregar BULTOS en donde solo debes agregar medidas y peso" sqref="A8:A169" xr:uid="{00000000-0002-0000-0000-00001F000000}">
       <formula1>"EMISION, BULTO"</formula1>
     </dataValidation>
     <dataValidation type="whole" allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Debes ingresar el teléfono del destinatario 9 dígitos" sqref="F8:F1048576" xr:uid="{0A81580A-1FF0-E34B-8D2B-13D1BB0FDA23}">

</xml_diff>